<commit_message>
Calender showing all task
</commit_message>
<xml_diff>
--- a/pathWay.xlsx
+++ b/pathWay.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nira\EmployeeManagementFrontEnd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37B73EC-A418-426F-B2A3-AB85B0D1423D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56E7EB4-0709-404B-AE38-5682B03AFC16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F1C29D8D-B93D-4747-9A8A-C389FA850BD7}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
   <si>
     <t>Page/</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>TaskBar.js</t>
+  </si>
+  <si>
+    <t>AllTaskCalendar</t>
   </si>
 </sst>
 </file>
@@ -601,11 +604,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEE03752-506D-4C0E-B5AD-D6DCEAD4A98B}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -829,6 +832,11 @@
         <v>35</v>
       </c>
     </row>
+    <row r="28" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>